<commit_message>
Add updated self evaluation files
</commit_message>
<xml_diff>
--- a/docs/auto-avaliacao-075.xlsx
+++ b/docs/auto-avaliacao-075.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\usr\ist\2023_2024_UC_RC\Lab\Proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F439A6C1-802A-4EFC-9FA6-B6F6847F621D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC26906-CEC1-4969-ACFF-59ABAE41F620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19545" yWindow="-16530" windowWidth="16200" windowHeight="16875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13440" yWindow="-15510" windowWidth="16200" windowHeight="13220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Autoavaliação" sheetId="1" r:id="rId1"/>
@@ -535,7 +535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
@@ -596,6 +596,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -930,7 +933,7 @@
   <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -961,11 +964,11 @@
       </c>
       <c r="B3" s="9"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="23"/>
     </row>
     <row r="5" spans="1:7" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="10" t="s">
@@ -1485,7 +1488,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="1148" yWindow="835" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="1148" yWindow="835" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="erro" error="dados inválidos" promptTitle="cotação" prompt="cotação" xr:uid="{F0D03626-1361-4688-8381-BA945540647D}">
           <x14:formula1>
             <xm:f>lists!$F$3:$F$7</xm:f>
@@ -1503,12 +1506,6 @@
             <xm:f>lists!$J$3:$J$6</xm:f>
           </x14:formula1>
           <xm:sqref>B32:B55</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Turno" prompt="Escolha o seu turno" xr:uid="{2C13F16D-5893-4173-8686-EA4B377B9FF9}">
-          <x14:formula1>
-            <xm:f>lists!$B$3:$B$15</xm:f>
-          </x14:formula1>
-          <xm:sqref>B4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="cotação" prompt="cotação" xr:uid="{FF51019F-7303-4EF2-B987-17BA5BCF754C}">
           <x14:formula1>

</xml_diff>

<commit_message>
Updata self evaluation excel
</commit_message>
<xml_diff>
--- a/docs/auto-avaliacao-075.xlsx
+++ b/docs/auto-avaliacao-075.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\usr\ist\2023_2024_UC_RC\Lab\Proj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raquel\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC26906-CEC1-4969-ACFF-59ABAE41F620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152DB957-CDA4-4979-8D94-9F6A006E7CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13440" yWindow="-15510" windowWidth="16200" windowHeight="13220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Autoavaliação" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="93">
   <si>
     <t>Ficha de autoavaliação</t>
   </si>
@@ -384,6 +384,9 @@
   </si>
   <si>
     <t>script 15</t>
+  </si>
+  <si>
+    <t>RCL10</t>
   </si>
 </sst>
 </file>
@@ -585,6 +588,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -596,9 +602,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -933,50 +936,54 @@
   <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.796875" customWidth="1"/>
-    <col min="2" max="2" width="9.9296875" style="4" customWidth="1"/>
-    <col min="3" max="4" width="4.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="50.86328125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="9.9296875" customWidth="1"/>
-    <col min="7" max="7" width="6.06640625" customWidth="1"/>
+    <col min="1" max="1" width="47.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10" style="4" customWidth="1"/>
+    <col min="3" max="4" width="4.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="50.85546875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="19"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A2" s="19" t="s">
+      <c r="B1" s="20"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B2" s="20"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="9"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="23"/>
-    </row>
-    <row r="5" spans="1:7" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="11"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="B5" s="11">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="14" t="s">
         <v>16</v>
@@ -984,13 +991,13 @@
       <c r="E6" s="2"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:7" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="15">
         <f>B8+F8</f>
-        <v>0</v>
+        <v>19.75</v>
       </c>
       <c r="C7" s="4">
         <f>C8+G8</f>
@@ -1002,13 +1009,13 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>50</v>
       </c>
       <c r="B8" s="7">
         <f>SUM(B9:B27)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C8" s="4">
         <f>SUM(C9:C27)</f>
@@ -1019,126 +1026,154 @@
       </c>
       <c r="F8" s="7">
         <f>SUM(F9:F27)</f>
-        <v>0</v>
+        <v>7.75</v>
       </c>
       <c r="G8" s="4">
         <f>SUM(G9:G27)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="8">
+        <v>1</v>
+      </c>
       <c r="C9" s="4">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="8">
+        <v>0.25</v>
+      </c>
       <c r="G9" s="4">
         <v>0.25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="8">
+        <v>0.5</v>
+      </c>
       <c r="C10" s="4">
         <v>0.5</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="8">
+        <v>0.5</v>
+      </c>
       <c r="G10" s="4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="8">
+        <v>0.5</v>
+      </c>
       <c r="C11" s="4">
         <v>0.5</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="8">
+        <v>0.5</v>
+      </c>
       <c r="G11" s="4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="8">
+        <v>1</v>
+      </c>
       <c r="C12" s="4">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="8"/>
+      <c r="F12" s="8">
+        <v>0.75</v>
+      </c>
       <c r="G12" s="4">
         <v>0.75</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="8">
+        <v>1</v>
+      </c>
       <c r="C13" s="4">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="8">
+        <v>1</v>
+      </c>
       <c r="G13" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="8">
+        <v>0.25</v>
+      </c>
       <c r="C14" s="4">
         <v>0.25</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="8"/>
+      <c r="F14" s="8">
+        <v>0.25</v>
+      </c>
       <c r="G14" s="4">
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="8">
+        <v>0.25</v>
+      </c>
       <c r="C15" s="4">
         <v>0.25</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F15" s="8"/>
+      <c r="F15" s="8">
+        <v>0.25</v>
+      </c>
       <c r="G15" s="4">
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -1148,28 +1183,32 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="11"/>
+      <c r="B17" s="11">
+        <v>1.5</v>
+      </c>
       <c r="C17" s="4">
         <v>1.5</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F17" s="8"/>
+      <c r="F17" s="8">
+        <v>1</v>
+      </c>
       <c r="G17" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E18" s="1"/>
       <c r="F18" s="7"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>34</v>
       </c>
@@ -1180,7 +1219,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -1190,71 +1229,87 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="11"/>
+      <c r="B21" s="11">
+        <v>2</v>
+      </c>
       <c r="C21" s="4">
         <v>2</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F21" s="8"/>
+      <c r="F21" s="8">
+        <v>0.75</v>
+      </c>
       <c r="G21" s="4">
         <v>0.75</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="8"/>
+      <c r="B22" s="8">
+        <v>0.5</v>
+      </c>
       <c r="C22" s="18">
         <v>0.5</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F22" s="8"/>
+      <c r="F22" s="8">
+        <v>0.5</v>
+      </c>
       <c r="G22" s="4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="8"/>
+      <c r="B23" s="8">
+        <v>1</v>
+      </c>
       <c r="C23" s="4">
         <v>1</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F23" s="8"/>
+      <c r="F23" s="8">
+        <v>0.75</v>
+      </c>
       <c r="G23" s="4">
         <v>0.75</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="8"/>
+      <c r="B24" s="8">
+        <v>0.5</v>
+      </c>
       <c r="C24" s="4">
         <v>0.5</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F24" s="8"/>
+      <c r="F24" s="8">
+        <v>0.5</v>
+      </c>
       <c r="G24" s="4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -1263,218 +1318,270 @@
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="11"/>
+      <c r="B26" s="11">
+        <v>2</v>
+      </c>
       <c r="C26" s="4">
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F26" s="8"/>
+      <c r="F26" s="8">
+        <v>0.75</v>
+      </c>
       <c r="G26" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="43.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="20"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="22"/>
-    </row>
-    <row r="30" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:7" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="21"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="23"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="12"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="8"/>
+      <c r="B32" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="8"/>
+      <c r="B33" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="8"/>
+      <c r="B34" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="8"/>
+      <c r="B35" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="8"/>
+      <c r="B36" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="8"/>
+      <c r="B37" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B38" s="8"/>
+      <c r="B38" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G38" s="4"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B39" s="8"/>
+      <c r="B39" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G39" s="4"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="8"/>
+      <c r="B40" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B41" s="8"/>
+      <c r="B41" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G41" s="4"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="8"/>
+      <c r="B42" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G42" s="4"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B43" s="8"/>
+      <c r="B43" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G43" s="4"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="8"/>
+      <c r="B44" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G44" s="4"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B45" s="8"/>
+      <c r="B45" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G45" s="4"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B46" s="8"/>
+      <c r="B46" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G46" s="4"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B47" s="8"/>
+      <c r="B47" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G47" s="4"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B48" s="8"/>
+      <c r="B48" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G48" s="4"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B49" s="8"/>
+      <c r="B49" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G49" s="4"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B50" s="8"/>
+      <c r="B50" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G50" s="4"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="8"/>
+      <c r="B51" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G51" s="4"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B52" s="8"/>
+      <c r="B52" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G52" s="4"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B53" s="8"/>
+      <c r="B53" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G53" s="4"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B54" s="8"/>
+      <c r="B54" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G54" s="4"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B55" s="8"/>
+      <c r="B55" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G55" s="4"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="16"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="16"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="16"/>
     </row>
   </sheetData>
@@ -1527,13 +1634,13 @@
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.796875" customWidth="1"/>
-    <col min="10" max="10" width="9.9296875" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>14</v>
       </c>
@@ -1550,7 +1657,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>35</v>
       </c>
@@ -1567,7 +1674,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>36</v>
       </c>
@@ -1584,7 +1691,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>37</v>
       </c>
@@ -1601,7 +1708,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>38</v>
       </c>
@@ -1615,7 +1722,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>39</v>
       </c>
@@ -1626,7 +1733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>40</v>
       </c>
@@ -1634,7 +1741,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>41</v>
       </c>
@@ -1642,7 +1749,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>42</v>
       </c>
@@ -1650,7 +1757,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>43</v>
       </c>
@@ -1658,22 +1765,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>47</v>
       </c>

</xml_diff>